<commit_message>
Inclusão da análise do Alpha
</commit_message>
<xml_diff>
--- a/arquivos/perguntas-questionario.xlsx
+++ b/arquivos/perguntas-questionario.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\demet\git\ppca-engenharia-requisitos\arquivos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42B69D74-4A27-4F0D-8CB4-2DF47BB903FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6848BFD-B744-4DDB-9BAE-3D76D90CA8F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19320" yWindow="-1050" windowWidth="19440" windowHeight="10440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -1050,8 +1050,8 @@
   </sheetPr>
   <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="F41" sqref="F41"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1059,7 +1059,7 @@
     <col min="1" max="1" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="4" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="54.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="204" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Separação do formulário de conhecimento e metodos
</commit_message>
<xml_diff>
--- a/arquivos/perguntas-questionario.xlsx
+++ b/arquivos/perguntas-questionario.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\demet\git\ppca-engenharia-requisitos\arquivos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6848BFD-B744-4DDB-9BAE-3D76D90CA8F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FFB7917-8404-4215-A91D-452474F92E57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-19320" yWindow="-1050" windowWidth="19440" windowHeight="10440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="88">
   <si>
     <t>id</t>
   </si>
@@ -138,15 +138,9 @@
     <t>Qual seu nível de conhecimento acerca dos temas abaixo? [Sprint de desenvolvimento de solução]</t>
   </si>
   <si>
-    <t>Metodologia</t>
-  </si>
-  <si>
     <t>Qual seu nível de conhecimento acerca dos temas abaixo? [Cascata ]</t>
   </si>
   <si>
-    <t>Conceito</t>
-  </si>
-  <si>
     <t>Qual seu nível de conhecimento acerca dos temas abaixo? [Engenharia de Requisitos]</t>
   </si>
   <si>
@@ -301,6 +295,9 @@
   </si>
   <si>
     <t>Percepções sobre gestão de requisitos. 1 indica que você discorda totalmente e 5, que você concorda completamente.  [Creio que realizar as atividades de gestão de requisitos é importante porque ela pode ajudar a entregar melhores funcionalidades]</t>
+  </si>
+  <si>
+    <t>QMC</t>
   </si>
 </sst>
 </file>
@@ -789,52 +786,52 @@
         <v>20</v>
       </c>
       <c r="Y1" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="Z1" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="Z1" s="3" t="s">
+      <c r="AA1" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB1" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="AA1" s="3" t="s">
+      <c r="AC1" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="AB1" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="AC1" s="3" t="s">
-        <v>40</v>
-      </c>
       <c r="AD1" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="AE1" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="AE1" s="3" t="s">
-        <v>45</v>
-      </c>
       <c r="AF1" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="AG1" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="AH1" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="AG1" s="3" t="s">
+      <c r="AI1" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="AH1" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="AI1" s="3" t="s">
+      <c r="AJ1" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="AJ1" s="3" t="s">
+      <c r="AK1" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="AL1" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="AK1" s="3" t="s">
+      <c r="AM1" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="AL1" s="3" t="s">
+      <c r="AN1" s="4" t="s">
         <v>55</v>
-      </c>
-      <c r="AM1" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="AN1" s="4" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:40" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -960,82 +957,82 @@
     </row>
     <row r="26" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="27" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="28" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="29" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="30" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="31" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="32" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="33" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="34" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="35" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="36" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="37" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="38" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="39" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="40" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="41" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -1050,8 +1047,8 @@
   </sheetPr>
   <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1167,7 +1164,7 @@
         <v>6</v>
       </c>
       <c r="F9" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1192,7 +1189,7 @@
         <v>17</v>
       </c>
       <c r="F11" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1206,7 +1203,7 @@
         <v>19</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1220,7 +1217,7 @@
         <v>19</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1234,7 +1231,7 @@
         <v>19</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1248,7 +1245,7 @@
         <v>23</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1262,7 +1259,7 @@
         <v>17</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1276,7 +1273,7 @@
         <v>23</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1290,7 +1287,7 @@
         <v>17</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1304,7 +1301,7 @@
         <v>23</v>
       </c>
       <c r="F19" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1318,7 +1315,7 @@
         <v>23</v>
       </c>
       <c r="F20" s="6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1332,7 +1329,7 @@
         <v>17</v>
       </c>
       <c r="F21" s="6" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1346,7 +1343,7 @@
         <v>17</v>
       </c>
       <c r="F22" s="6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1360,7 +1357,7 @@
         <v>17</v>
       </c>
       <c r="F23" s="6" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1374,7 +1371,7 @@
         <v>19</v>
       </c>
       <c r="F24" s="6" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1388,7 +1385,7 @@
         <v>19</v>
       </c>
       <c r="F25" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1396,13 +1393,10 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>16</v>
-      </c>
-      <c r="E26" t="s">
-        <v>34</v>
+        <v>87</v>
       </c>
       <c r="F26" s="6" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1410,13 +1404,10 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>16</v>
-      </c>
-      <c r="E27" t="s">
-        <v>36</v>
+        <v>87</v>
       </c>
       <c r="F27" s="6" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1424,13 +1415,10 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>16</v>
-      </c>
-      <c r="E28" t="s">
-        <v>34</v>
+        <v>87</v>
       </c>
       <c r="F28" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1438,13 +1426,10 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>16</v>
-      </c>
-      <c r="E29" t="s">
-        <v>34</v>
+        <v>87</v>
       </c>
       <c r="F29" s="6" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1452,13 +1437,10 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>16</v>
-      </c>
-      <c r="E30" t="s">
-        <v>34</v>
+        <v>87</v>
       </c>
       <c r="F30" s="6" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1466,13 +1448,13 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C31" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F31" s="6" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1480,13 +1462,13 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C32" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F32" s="6" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1494,16 +1476,16 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C33" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D33" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F33" s="6" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1511,13 +1493,13 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C34" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F34" s="6" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1525,13 +1507,13 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C35" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F35" s="6" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1539,16 +1521,16 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C36" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D36" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F36" s="6" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1556,13 +1538,13 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C37" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F37" s="6" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1570,16 +1552,16 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C38" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D38" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F38" s="6" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1587,16 +1569,16 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C39" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D39" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F39" s="6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1604,13 +1586,13 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C40" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F40" s="6" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="41" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1618,13 +1600,13 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C41" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F41" s="6" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>

</xml_diff>